<commit_message>
add get ntc temp and mute/unmute amp,update lvp15 excel
</commit_message>
<xml_diff>
--- a/lvp15_test_command_list_tag1.0.xlsx
+++ b/lvp15_test_command_list_tag1.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="135">
   <si>
     <t>No.</t>
   </si>
@@ -476,6 +476,76 @@
   </si>
   <si>
     <t>press for one second and then run this script,get the touch counter.this script just support cypress widget, mute\mufunction\pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./ntc_temp_get.sh &lt;ntc_addr&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ntc_temp_get.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/ntc_temp_get.sh 0x48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/ntc_temp_get.sh 0x49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/ntc_temp_get.sh 0x4a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/ntc_temp_get.sh 0x4b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">get the 0x48 ntc temperature </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the 0x49 ntc temperature</t>
+  </si>
+  <si>
+    <t>get the 0x4a ntc temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the 0x4b ntc temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set_amp_mute.sh</t>
+  </si>
+  <si>
+    <t>set_amp_unmute.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./set_amp_mute.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/set_amp_mute.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/set_amp_unmute.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mute amp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unmute amp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./set_amp_unmute.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -499,7 +569,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +579,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,11 +601,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -834,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1347,6 +1424,108 @@
         <v>116</v>
       </c>
     </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" s="2">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add description for get_gsensor_direction.sh
</commit_message>
<xml_diff>
--- a/lvp15_test_command_list_tag1.0.xlsx
+++ b/lvp15_test_command_list_tag1.0.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="151">
   <si>
     <t>No.</t>
   </si>
@@ -593,6 +593,22 @@
   </si>
   <si>
     <t>adb shell /etc/factory-test/lvp15/get_sw_version.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_gsensor_direction.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./get_gsensor_direction.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/get_gsensor_direction.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get the direction of the devices through gsensor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -960,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1628,6 +1644,18 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" t="s">
+        <v>149</v>
+      </c>
+      <c r="E40" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41">

</xml_diff>

<commit_message>
add get/set DSN & MODULE_SN scripts & modified test command list
</commit_message>
<xml_diff>
--- a/lvp15_test_command_list_tag1.0.xlsx
+++ b/lvp15_test_command_list_tag1.0.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="170">
   <si>
     <t>No.</t>
   </si>
@@ -625,25 +625,78 @@
   <si>
     <t>./button_f_check.sh cypress</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_DSN.sh</t>
+  </si>
+  <si>
+    <t>get_MODULE_SN.sh</t>
+  </si>
+  <si>
+    <t>set_DSN.sh</t>
+  </si>
+  <si>
+    <t>set_MODULE_SN.sh</t>
+  </si>
+  <si>
+    <t>./get_DSN.sh</t>
+  </si>
+  <si>
+    <t>./get_MODULE_SN.sh</t>
+  </si>
+  <si>
+    <t>./set_DSN.sh</t>
+  </si>
+  <si>
+    <t>./set_MODULE_SN.sh</t>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/get_MODULE_SN.sh</t>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/get_DSN.sh</t>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/set_DSN.sh 1234</t>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/lvp15/set_MODULE_SN.sh ZTQ03M130144</t>
+  </si>
+  <si>
+    <t>get Device serial number</t>
+  </si>
+  <si>
+    <t>get Moduel serial number</t>
+  </si>
+  <si>
+    <t>if success return OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -679,15 +732,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -703,7 +758,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -991,20 +1046,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="25.75" customWidth="1"/>
-    <col min="3" max="3" width="45.375" customWidth="1"/>
-    <col min="4" max="4" width="83.75" customWidth="1"/>
-    <col min="5" max="5" width="98.75" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="83.7109375" customWidth="1"/>
+    <col min="5" max="5" width="98.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1076,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1038,7 +1093,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1055,7 +1110,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1072,7 +1127,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1089,7 +1144,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1106,7 +1161,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1123,7 +1178,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1140,7 +1195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1157,7 +1212,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1174,7 +1229,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1191,7 +1246,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1208,7 +1263,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1225,7 +1280,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1242,7 +1297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1259,7 +1314,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1276,7 +1331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1293,7 +1348,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1307,35 +1362,35 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19">
+    <row r="19" spans="1:5" s="3" customFormat="1">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20">
+    <row r="20" spans="1:5" s="3" customFormat="1">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1352,7 +1407,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1369,7 +1424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1383,7 +1438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1400,7 +1455,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1417,7 +1472,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1434,7 +1489,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1451,7 +1506,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1468,7 +1523,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1485,7 +1540,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1502,7 +1557,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" s="2" customFormat="1">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1519,7 +1574,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" s="2" customFormat="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1536,41 +1591,41 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33">
+    <row r="33" spans="1:5" s="4" customFormat="1">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A34">
+    <row r="34" spans="1:5" s="4" customFormat="1">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1587,7 +1642,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1604,7 +1659,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1621,7 +1676,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1638,7 +1693,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1655,131 +1710,179 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40">
+    <row r="40" spans="1:5" s="3" customFormat="1">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41">
+    <row r="41" spans="1:5" s="3" customFormat="1">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" t="s">
+        <v>159</v>
+      </c>
+      <c r="D42" t="s">
+        <v>164</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B43" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B45" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:1">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:1">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:1">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:1">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:1">
       <c r="A60">
         <v>59</v>
       </c>

</xml_diff>